<commit_message>
create criteria and tension tests and implementation
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162850FC-C6B5-48AE-841C-48732594F75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801FD2BF-AC0A-471E-8EEA-5533560F20DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1700" windowWidth="14400" windowHeight="7280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
+    <sheet name="Tension" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Secao</t>
   </si>
@@ -72,6 +73,42 @@
   </si>
   <si>
     <t>Web flexural slender limit</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>gross area</t>
+  </si>
+  <si>
+    <t>net area</t>
+  </si>
+  <si>
+    <t>yield strength Mpa</t>
+  </si>
+  <si>
+    <t>ultimate strength Mpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lag factor </t>
+  </si>
+  <si>
+    <t>effective are</t>
+  </si>
+  <si>
+    <t>w6x15</t>
+  </si>
+  <si>
+    <t>nominal ult str</t>
+  </si>
+  <si>
+    <t>nominal yield strength</t>
+  </si>
+  <si>
+    <t>ultimate strength lrfd</t>
+  </si>
+  <si>
+    <t>yield strength lrfd</t>
   </si>
 </sst>
 </file>
@@ -392,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,4 +524,102 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Trebuchet MS"&amp;9&amp;K737373 PÚBLICA</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3679AAC7-575D-4078-88D0-2A2187398AB4}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>355</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>2860</v>
+      </c>
+      <c r="E2">
+        <v>2860</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>F2*E2</f>
+        <v>2860</v>
+      </c>
+      <c r="H2">
+        <f>G2*B2</f>
+        <v>1430000</v>
+      </c>
+      <c r="I2">
+        <f>D2*A2</f>
+        <v>1015300</v>
+      </c>
+      <c r="J2">
+        <f>H2*0.75</f>
+        <v>1072500</v>
+      </c>
+      <c r="K2">
+        <f>0.9*I2</f>
+        <v>913770</v>
+      </c>
+      <c r="L2">
+        <f>H2/2</f>
+        <v>715000</v>
+      </c>
+      <c r="M2">
+        <f>I2/1.67</f>
+        <v>607964.07185628742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor and add compression failing test
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801FD2BF-AC0A-471E-8EEA-5533560F20DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899EA715-F77A-4EF1-B333-63708B8C9839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1700" windowWidth="14400" windowHeight="7280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
     <sheet name="Tension" sheetId="2" r:id="rId2"/>
+    <sheet name="Compression" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Secao</t>
   </si>
@@ -109,6 +110,60 @@
   </si>
   <si>
     <t>yield strength lrfd</t>
+  </si>
+  <si>
+    <t>ult str asd</t>
+  </si>
+  <si>
+    <t>yield str asd</t>
+  </si>
+  <si>
+    <t>Linear modulus E GPa</t>
+  </si>
+  <si>
+    <t>Yield Strength Fy MPa</t>
+  </si>
+  <si>
+    <t>radius gyration x (mm)</t>
+  </si>
+  <si>
+    <t>radius gyration y (mm)</t>
+  </si>
+  <si>
+    <t>Gross Area Ag (mm2)</t>
+  </si>
+  <si>
+    <t>length x (m)</t>
+  </si>
+  <si>
+    <t>length y (m)</t>
+  </si>
+  <si>
+    <t>l/r x</t>
+  </si>
+  <si>
+    <t>l/r y</t>
+  </si>
+  <si>
+    <t>elastic buckling stress FE  x (MPa)</t>
+  </si>
+  <si>
+    <t>Fy/Fe x</t>
+  </si>
+  <si>
+    <t>elastic buckling stress FE  y (MPa)</t>
+  </si>
+  <si>
+    <t>critical stress x 1</t>
+  </si>
+  <si>
+    <t>Fy/Fe y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">critical stress x 2 </t>
+  </si>
+  <si>
+    <t>criticak stress 1</t>
   </si>
 </sst>
 </file>
@@ -530,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3679AAC7-575D-4078-88D0-2A2187398AB4}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,6 +625,12 @@
       <c r="K1" t="s">
         <v>23</v>
       </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -617,6 +678,170 @@
       <c r="M2">
         <f>I2/1.67</f>
         <v>607964.07185628742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66988232-ECD8-43F1-9F3B-FF1388B8657D}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="18.6328125" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
+    <col min="11" max="14" width="18.7265625" customWidth="1"/>
+    <col min="15" max="15" width="32.08984375" customWidth="1"/>
+    <col min="16" max="16" width="20.453125" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" customWidth="1"/>
+    <col min="19" max="19" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>200</v>
+      </c>
+      <c r="B2">
+        <v>355</v>
+      </c>
+      <c r="C2">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E2">
+        <v>2860</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>F2*1000/C2</f>
+        <v>15.384615384615385</v>
+      </c>
+      <c r="I2">
+        <f>G2*1000/D2</f>
+        <v>27.173913043478262</v>
+      </c>
+      <c r="J2">
+        <f>A2*PI()^2/(F2*1000/C2)^2*1000</f>
+        <v>8339.8157189205067</v>
+      </c>
+      <c r="K2">
+        <f>B2/J2</f>
+        <v>4.2566887802402267E-2</v>
+      </c>
+      <c r="L2">
+        <f>0.658^K2*B2</f>
+        <v>348.73119264684101</v>
+      </c>
+      <c r="M2">
+        <f>0.877*J2</f>
+        <v>7314.0183854932848</v>
+      </c>
+      <c r="N2">
+        <f>IF(K2&lt;=2.25,1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <f>A2*PI()^2/(G2*1000/D2)^2*1000</f>
+        <v>2673.1626128262501</v>
+      </c>
+      <c r="P2">
+        <f>B2/O2</f>
+        <v>0.13280149823159085</v>
+      </c>
+      <c r="Q2">
+        <f>0.658^P2*B2</f>
+        <v>335.80602147781121</v>
+      </c>
+      <c r="R2">
+        <f>0.877*O2</f>
+        <v>2344.3636114486212</v>
+      </c>
+      <c r="S2">
+        <f>IF(P2&lt;=2.25,1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include minor axis flexural buckling calculation with passing tests
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899EA715-F77A-4EF1-B333-63708B8C9839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E2070-8801-4E92-8945-440A9F55A264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Secao</t>
   </si>
@@ -163,15 +163,41 @@
     <t xml:space="preserve">critical stress x 2 </t>
   </si>
   <si>
-    <t>criticak stress 1</t>
+    <t>k x</t>
+  </si>
+  <si>
+    <t>ky</t>
+  </si>
+  <si>
+    <t>nominal strength</t>
+  </si>
+  <si>
+    <t>design strength</t>
+  </si>
+  <si>
+    <t>criticak stress</t>
+  </si>
+  <si>
+    <t>critical stress y 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">critical stress y 2 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,9 +225,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,10 +714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66988232-ECD8-43F1-9F3B-FF1388B8657D}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,17 +726,17 @@
     <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="18.6328125" customWidth="1"/>
-    <col min="10" max="10" width="32" customWidth="1"/>
-    <col min="11" max="14" width="18.7265625" customWidth="1"/>
-    <col min="15" max="15" width="32.08984375" customWidth="1"/>
-    <col min="16" max="16" width="20.453125" customWidth="1"/>
-    <col min="17" max="17" width="15.54296875" customWidth="1"/>
-    <col min="18" max="18" width="17.1796875" customWidth="1"/>
-    <col min="19" max="19" width="16.08984375" customWidth="1"/>
+    <col min="6" max="11" width="18.6328125" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="13" max="18" width="18.7265625" customWidth="1"/>
+    <col min="19" max="19" width="32.08984375" customWidth="1"/>
+    <col min="20" max="20" width="20.453125" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
+    <col min="22" max="22" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -726,49 +753,67 @@
         <v>30</v>
       </c>
       <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" t="s">
         <v>37</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
+      <c r="U1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>200</v>
       </c>
@@ -791,60 +836,81 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <f>F2*1000/C2</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>G2*1000/C2</f>
         <v>15.384615384615385</v>
       </c>
-      <c r="I2">
-        <f>G2*1000/D2</f>
+      <c r="K2">
+        <f>I2*1000/D2</f>
         <v>27.173913043478262</v>
       </c>
-      <c r="J2">
-        <f>A2*PI()^2/(F2*1000/C2)^2*1000</f>
+      <c r="L2">
+        <f>A2*PI()^2/(F2*G2*1000/C2)^2*1000</f>
         <v>8339.8157189205067</v>
       </c>
-      <c r="K2">
-        <f>B2/J2</f>
+      <c r="M2">
+        <f>B2/L2</f>
         <v>4.2566887802402267E-2</v>
       </c>
-      <c r="L2">
-        <f>0.658^K2*B2</f>
+      <c r="N2">
+        <f>0.658^M2*B2</f>
         <v>348.73119264684101</v>
       </c>
-      <c r="M2">
-        <f>0.877*J2</f>
+      <c r="O2">
+        <f>0.877*L2</f>
         <v>7314.0183854932848</v>
       </c>
-      <c r="N2">
-        <f>IF(K2&lt;=2.25,1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <f>A2*PI()^2/(G2*1000/D2)^2*1000</f>
+      <c r="P2">
+        <f>IF(M2&lt;=2.25,N2,O2)</f>
+        <v>348.73119264684101</v>
+      </c>
+      <c r="Q2">
+        <f>P2*E2</f>
+        <v>997371.21096996532</v>
+      </c>
+      <c r="R2">
+        <f>Q2/1.67</f>
+        <v>597228.27004189545</v>
+      </c>
+      <c r="S2">
+        <f>A2*PI()^2/(H2*I2*1000/D2)^2*1000</f>
         <v>2673.1626128262501</v>
       </c>
-      <c r="P2">
-        <f>B2/O2</f>
+      <c r="T2">
+        <f>B2/S2</f>
         <v>0.13280149823159085</v>
       </c>
-      <c r="Q2">
-        <f>0.658^P2*B2</f>
+      <c r="U2">
+        <f>0.658^T2*B2</f>
         <v>335.80602147781121</v>
       </c>
-      <c r="R2">
-        <f>0.877*O2</f>
+      <c r="V2">
+        <f>0.877*S2</f>
         <v>2344.3636114486212</v>
       </c>
-      <c r="S2">
-        <f>IF(P2&lt;=2.25,1,2)</f>
-        <v>1</v>
+      <c r="W2">
+        <f>IF(T2&lt;=2.25,U2,V2)</f>
+        <v>335.80602147781121</v>
+      </c>
+      <c r="X2">
+        <f>W2*E2</f>
+        <v>960405.22142654005</v>
+      </c>
+      <c r="Y2">
+        <f>X2/1.67</f>
+        <v>575092.9469620001</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="Q5">
-        <v>6</v>
-      </c>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor tension calculation and tests
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E2070-8801-4E92-8945-440A9F55A264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D6FD8-8273-4070-84F8-88E108F5CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="21150" yWindow="1710" windowWidth="14300" windowHeight="7140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
     <sheet name="Tension" sheetId="2" r:id="rId2"/>
     <sheet name="Compression" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Secao</t>
   </si>
@@ -182,6 +183,30 @@
   </si>
   <si>
     <t xml:space="preserve">critical stress y 2 </t>
+  </si>
+  <si>
+    <t>elastic torsional stress</t>
+  </si>
+  <si>
+    <t>inertia x</t>
+  </si>
+  <si>
+    <t>inertia y</t>
+  </si>
+  <si>
+    <t>torsional constant</t>
+  </si>
+  <si>
+    <t>warping constant</t>
+  </si>
+  <si>
+    <t>Shear Modulus Gpa</t>
+  </si>
+  <si>
+    <t>length torsion</t>
+  </si>
+  <si>
+    <t>k torsion</t>
   </si>
 </sst>
 </file>
@@ -714,94 +739,99 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66988232-ECD8-43F1-9F3B-FF1388B8657D}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="18.6328125" customWidth="1"/>
-    <col min="12" max="12" width="32" customWidth="1"/>
-    <col min="13" max="18" width="18.7265625" customWidth="1"/>
-    <col min="19" max="19" width="32.08984375" customWidth="1"/>
-    <col min="20" max="20" width="20.453125" customWidth="1"/>
-    <col min="21" max="21" width="15.54296875" customWidth="1"/>
-    <col min="22" max="22" width="17.1796875" customWidth="1"/>
-    <col min="23" max="23" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="18.90625" customWidth="1"/>
+    <col min="8" max="9" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="18.6328125" customWidth="1"/>
+    <col min="19" max="19" width="32" customWidth="1"/>
+    <col min="20" max="25" width="18.7265625" customWidth="1"/>
+    <col min="26" max="26" width="32.08984375" customWidth="1"/>
+    <col min="27" max="27" width="20.453125" customWidth="1"/>
+    <col min="28" max="28" width="15.54296875" customWidth="1"/>
+    <col min="29" max="29" width="17.1796875" customWidth="1"/>
+    <col min="30" max="30" width="16.08984375" customWidth="1"/>
+    <col min="34" max="34" width="39.54296875" customWidth="1"/>
+    <col min="35" max="35" width="13.7265625" customWidth="1"/>
+    <col min="36" max="36" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" t="s">
-        <v>47</v>
       </c>
       <c r="W1" t="s">
         <v>45</v>
@@ -812,105 +842,212 @@
       <c r="Y1" t="s">
         <v>44</v>
       </c>
+      <c r="Z1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>200</v>
       </c>
       <c r="B2">
+        <v>77</v>
+      </c>
+      <c r="C2">
         <v>355</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>12.1</v>
+      </c>
+      <c r="E2">
+        <v>3.88</v>
+      </c>
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>20.5</v>
+      </c>
+      <c r="H2">
         <v>65</v>
       </c>
-      <c r="D2">
+      <c r="I2">
         <v>36.799999999999997</v>
       </c>
-      <c r="E2">
+      <c r="J2">
         <v>2860</v>
       </c>
-      <c r="F2">
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <f>G2*1000/C2</f>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <f>L2*1000/H2</f>
         <v>15.384615384615385</v>
       </c>
-      <c r="K2">
-        <f>I2*1000/D2</f>
+      <c r="R2">
+        <f>N2*1000/I2</f>
         <v>27.173913043478262</v>
       </c>
-      <c r="L2">
-        <f>A2*PI()^2/(F2*G2*1000/C2)^2*1000</f>
+      <c r="S2">
+        <f>A2*PI()^2/(K2*L2*1000/H2)^2*1000</f>
         <v>8339.8157189205067</v>
       </c>
-      <c r="M2">
-        <f>B2/L2</f>
+      <c r="T2">
+        <f>C2/S2</f>
         <v>4.2566887802402267E-2</v>
       </c>
-      <c r="N2">
-        <f>0.658^M2*B2</f>
+      <c r="U2">
+        <f>0.658^T2*C2</f>
         <v>348.73119264684101</v>
-      </c>
-      <c r="O2">
-        <f>0.877*L2</f>
-        <v>7314.0183854932848</v>
-      </c>
-      <c r="P2">
-        <f>IF(M2&lt;=2.25,N2,O2)</f>
-        <v>348.73119264684101</v>
-      </c>
-      <c r="Q2">
-        <f>P2*E2</f>
-        <v>997371.21096996532</v>
-      </c>
-      <c r="R2">
-        <f>Q2/1.67</f>
-        <v>597228.27004189545</v>
-      </c>
-      <c r="S2">
-        <f>A2*PI()^2/(H2*I2*1000/D2)^2*1000</f>
-        <v>2673.1626128262501</v>
-      </c>
-      <c r="T2">
-        <f>B2/S2</f>
-        <v>0.13280149823159085</v>
-      </c>
-      <c r="U2">
-        <f>0.658^T2*B2</f>
-        <v>335.80602147781121</v>
       </c>
       <c r="V2">
         <f>0.877*S2</f>
-        <v>2344.3636114486212</v>
+        <v>7314.0183854932848</v>
       </c>
       <c r="W2">
         <f>IF(T2&lt;=2.25,U2,V2)</f>
-        <v>335.80602147781121</v>
+        <v>348.73119264684101</v>
       </c>
       <c r="X2">
-        <f>W2*E2</f>
-        <v>960405.22142654005</v>
+        <f>W2*J2</f>
+        <v>997371.21096996532</v>
       </c>
       <c r="Y2">
         <f>X2/1.67</f>
+        <v>597228.27004189545</v>
+      </c>
+      <c r="Z2">
+        <f>A2*PI()^2/(M2*N2*1000/I2)^2*1000</f>
+        <v>2673.1626128262501</v>
+      </c>
+      <c r="AA2">
+        <f>$C2/Z2</f>
+        <v>0.13280149823159085</v>
+      </c>
+      <c r="AB2">
+        <f>0.658^AA2*C2</f>
+        <v>335.80602147781121</v>
+      </c>
+      <c r="AC2">
+        <f>0.877*Z2</f>
+        <v>2344.3636114486212</v>
+      </c>
+      <c r="AD2">
+        <f>IF(AA2&lt;=2.25,AB2,AC2)</f>
+        <v>335.80602147781121</v>
+      </c>
+      <c r="AE2">
+        <f>AD2*$J2</f>
+        <v>960405.22142654005</v>
+      </c>
+      <c r="AF2">
+        <f>AE2/1.67</f>
         <v>575092.9469620001</v>
       </c>
+      <c r="AH2">
+        <f>(PI()^2*A2*10^3*G2*10^9/(P2*O2*1000)^2+B2*10^3*F2*10^3)*1/(D2*10^6+E2*10^6)</f>
+        <v>2734.6294145473321</v>
+      </c>
+      <c r="AI2">
+        <f>$C2/AH2</f>
+        <v>0.12981649290814923</v>
+      </c>
+      <c r="AJ2">
+        <f>0.658^AI2*C2</f>
+        <v>336.22583132658912</v>
+      </c>
+      <c r="AK2">
+        <f>0.877*AH2</f>
+        <v>2398.2699965580105</v>
+      </c>
+      <c r="AL2">
+        <f>IF(AI2&lt;=2.25,AJ2,AK2)</f>
+        <v>336.22583132658912</v>
+      </c>
+      <c r="AM2">
+        <f>AL2*$J2</f>
+        <v>961605.8775940449</v>
+      </c>
+      <c r="AN2">
+        <f>AM2/1.67</f>
+        <v>575811.90275092516</v>
+      </c>
+      <c r="AP2">
+        <f>(PI()^2*A2*10^3*G2*10^9/(P2*O2*1000)^2+B2*10^3*F2*10^3)</f>
+        <v>43699378044.46637</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="H3" s="2"/>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="M3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABFC60B-44BC-4DE3-8D59-3A6B316D4B1A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
include addtional flexure yielding test
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96D6FD8-8273-4070-84F8-88E108F5CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445BD9F1-39D0-4BBA-AAA4-A1D7B9D2F198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="21150" yWindow="1710" windowWidth="14300" windowHeight="7140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
     <sheet name="Tension" sheetId="2" r:id="rId2"/>
     <sheet name="Compression" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Flexure Major Axis" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>Secao</t>
   </si>
@@ -207,13 +207,28 @@
   </si>
   <si>
     <t>k torsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic section modulus </t>
+  </si>
+  <si>
+    <t>yield stress</t>
+  </si>
+  <si>
+    <t>nominal yielding strengt</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>design asd strength</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +243,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,10 +271,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66988232-ECD8-43F1-9F3B-FF1388B8657D}">
   <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
@@ -1042,12 +1066,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABFC60B-44BC-4DE3-8D59-3A6B316D4B1A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>26500</v>
+      </c>
+      <c r="C2">
+        <v>355</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>9407500</v>
+      </c>
+      <c r="E2">
+        <f>D2/1.67</f>
+        <v>5633233.532934132</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added i section flex test
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445BD9F1-39D0-4BBA-AAA4-A1D7B9D2F198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A653C-8BA2-4D43-88F9-6719EDA5F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
     <sheet name="Tension" sheetId="2" r:id="rId2"/>
     <sheet name="Compression" sheetId="3" r:id="rId3"/>
-    <sheet name="Flexure Major Axis" sheetId="4" r:id="rId4"/>
+    <sheet name="Flexure Major Axis Yield" sheetId="4" r:id="rId4"/>
+    <sheet name="Flex Maj Axis lat tor b" sheetId="5" r:id="rId5"/>
+    <sheet name="Flex Maj Axis lat tor c" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>Secao</t>
   </si>
@@ -215,13 +217,85 @@
     <t>yield stress</t>
   </si>
   <si>
-    <t>nominal yielding strengt</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>design asd strength</t>
+  </si>
+  <si>
+    <t>nominal yielding strength</t>
+  </si>
+  <si>
+    <t>elastic modulus Mpa</t>
+  </si>
+  <si>
+    <t>yield stress Mpa</t>
+  </si>
+  <si>
+    <t>Plastic section modulus mm3</t>
+  </si>
+  <si>
+    <t>Elastic seciton Modulus mm3</t>
+  </si>
+  <si>
+    <t>dist bet flage centroids mm</t>
+  </si>
+  <si>
+    <t>Torsional constant mm4</t>
+  </si>
+  <si>
+    <t>warping constant mm6</t>
+  </si>
+  <si>
+    <t>radius of gyration mm</t>
+  </si>
+  <si>
+    <t>minor axis inertia</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>inner root</t>
+  </si>
+  <si>
+    <t>outter root</t>
+  </si>
+  <si>
+    <t>eff radius</t>
+  </si>
+  <si>
+    <t>length lstral torsional buckling</t>
+  </si>
+  <si>
+    <t>liminting length yield</t>
+  </si>
+  <si>
+    <t>lemgth</t>
+  </si>
+  <si>
+    <t>plastic moment N mm</t>
+  </si>
+  <si>
+    <t>moment b N m</t>
+  </si>
+  <si>
+    <t>design moment</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>critical stress</t>
+  </si>
+  <si>
+    <t>desgin miment c</t>
   </si>
 </sst>
 </file>
@@ -271,13 +345,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,19 +1144,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABFC60B-44BC-4DE3-8D59-3A6B316D4B1A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
     <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -1089,10 +1168,10 @@
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1116,4 +1195,335 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C0A553-783A-45CB-94FE-504C3CB5AAEF}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U2" sqref="A1:U2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.1796875" customWidth="1"/>
+    <col min="19" max="19" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2100</v>
+      </c>
+      <c r="B2">
+        <v>200000</v>
+      </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
+      <c r="D2">
+        <v>177000</v>
+      </c>
+      <c r="E2">
+        <v>159000</v>
+      </c>
+      <c r="F2">
+        <v>146</v>
+      </c>
+      <c r="G2">
+        <v>42000</v>
+      </c>
+      <c r="H2" s="4">
+        <v>20500000000</v>
+      </c>
+      <c r="I2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J2">
+        <v>3880000</v>
+      </c>
+      <c r="L2">
+        <f>1.76 * I2 *(B2/C2)^0.5</f>
+        <v>1831.9156801556126</v>
+      </c>
+      <c r="M2" s="4">
+        <f>((J2*H2)^0.5/E2)^0.5</f>
+        <v>42.11606957892652</v>
+      </c>
+      <c r="N2">
+        <f>G2/(E2*F2)</f>
+        <v>1.8092530369604549E-3</v>
+      </c>
+      <c r="O2">
+        <f>(N2^2+6.76*(0.7*C2/B2)^2)^0.5</f>
+        <v>2.9067200676622831E-3</v>
+      </c>
+      <c r="P2">
+        <f>(N2+O2)^0.5</f>
+        <v>6.8672943031609895E-2</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>1.95*M2*B2/(0.7*C2)*P2</f>
+        <v>6445.5510531113505</v>
+      </c>
+      <c r="S2">
+        <f>D2*C2</f>
+        <v>44250000</v>
+      </c>
+      <c r="T2">
+        <f>(S2-(S2-0.7*C2*E2)*(A2-L2)/(Q2-L2))/1000</f>
+        <v>43295.593204167089</v>
+      </c>
+      <c r="U2">
+        <f>T2/1.67</f>
+        <v>25925.504912674904</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18661751-9BA2-4C4D-90C2-2BE11D0E00CC}">
+  <dimension ref="A2:Y3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.08984375" customWidth="1"/>
+    <col min="19" max="19" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.26953125" customWidth="1"/>
+    <col min="21" max="24" width="19.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7000</v>
+      </c>
+      <c r="B3">
+        <v>200000</v>
+      </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
+      <c r="D3">
+        <v>177000</v>
+      </c>
+      <c r="E3">
+        <v>159000</v>
+      </c>
+      <c r="F3">
+        <v>146</v>
+      </c>
+      <c r="G3">
+        <v>42000</v>
+      </c>
+      <c r="H3" s="4">
+        <v>20500000000</v>
+      </c>
+      <c r="I3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J3">
+        <v>3880000</v>
+      </c>
+      <c r="L3">
+        <f>1.76 * I3 *(B3/C3)^0.5</f>
+        <v>1831.9156801556126</v>
+      </c>
+      <c r="M3" s="4">
+        <f>((J3*H3)^0.5/E3)^0.5</f>
+        <v>42.11606957892652</v>
+      </c>
+      <c r="N3">
+        <f>G3/(E3*F3)</f>
+        <v>1.8092530369604549E-3</v>
+      </c>
+      <c r="O3">
+        <f>(N3^2+6.76*(0.7*C3/B3)^2)^0.5</f>
+        <v>2.9067200676622831E-3</v>
+      </c>
+      <c r="P3">
+        <f>(N3+O3)^0.5</f>
+        <v>6.8672943031609895E-2</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>1.95*M3*B3/(0.7*C3)*P3</f>
+        <v>6445.5510531113505</v>
+      </c>
+      <c r="S3">
+        <f>D3*C3</f>
+        <v>44250000</v>
+      </c>
+      <c r="U3" s="4">
+        <f>PI()^2*B3/(A3/M3)^2</f>
+        <v>71.454458113277298</v>
+      </c>
+      <c r="V3" s="4">
+        <f>(1+0.078*G3/(E3*F3)*(A3/M3)^2)^0.5</f>
+        <v>2.2132490018735647</v>
+      </c>
+      <c r="W3" s="4">
+        <f>V3*U3</f>
+        <v>158.14650809862741</v>
+      </c>
+      <c r="X3" s="5">
+        <f>W3*E3/1000</f>
+        <v>25145.29478768176</v>
+      </c>
+      <c r="Y3">
+        <f>X3/1.67</f>
+        <v>15057.062747114827</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add i section web shear check with test
</commit_message>
<xml_diff>
--- a/test/Manual Checks.xlsx
+++ b/test/Manual Checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U3ZO\GitRepos\struct_codes\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B36763-BC95-45D0-A7E8-718CD5AD3951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96458E-B685-48FF-930F-AA246FB01D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W profile slenderness" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Flex Maj Axis lat tor b" sheetId="5" r:id="rId5"/>
     <sheet name="Flex Maj Axis lat tor c" sheetId="6" r:id="rId6"/>
     <sheet name="Flex Minor Axis yield" sheetId="7" r:id="rId7"/>
+    <sheet name="Web Shear" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>Secao</t>
   </si>
@@ -315,6 +316,21 @@
   </si>
   <si>
     <t>nominal moment</t>
+  </si>
+  <si>
+    <t>web area mm</t>
+  </si>
+  <si>
+    <t>Elastic modulus MPa</t>
+  </si>
+  <si>
+    <t>web ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rolled web shear limit </t>
+  </si>
+  <si>
+    <t>web shear strength coefficient</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D32048-8704-470F-BAF4-ADF152211344}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1647,4 +1663,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A82D29-7830-4ED6-875D-2661E46C597C}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>200000</v>
+      </c>
+      <c r="B2">
+        <v>355</v>
+      </c>
+      <c r="C2">
+        <v>29344</v>
+      </c>
+      <c r="D2">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <f>2.24*(A2/B2)^0.5</f>
+        <v>53.167818287084629</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>0.6*B2*C2*F2</f>
+        <v>6250272</v>
+      </c>
+      <c r="H2">
+        <f>G2/1.5</f>
+        <v>4166848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>200000</v>
+      </c>
+      <c r="B3">
+        <v>250</v>
+      </c>
+      <c r="C3">
+        <v>887.68</v>
+      </c>
+      <c r="D3">
+        <v>21.6</v>
+      </c>
+      <c r="E3">
+        <f>2.24*(A3/B3)^0.5</f>
+        <v>63.356767594314668</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>0.6*B3*C3*F3</f>
+        <v>133152</v>
+      </c>
+      <c r="H3">
+        <f>G3</f>
+        <v>133152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>